<commit_message>
fixing dates and ages
</commit_message>
<xml_diff>
--- a/config/default/forms/app/child_assessment.xlsx
+++ b/config/default/forms/app/child_assessment.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1180" uniqueCount="589">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1184" uniqueCount="592">
   <si>
     <t>type</t>
   </si>
@@ -667,7 +667,7 @@
     <t>summary_age</t>
   </si>
   <si>
-    <t>${patient_age_in_years} years ${patient_age_in_months} months</t>
+    <t>${__display_age}</t>
   </si>
   <si>
     <t>summary_symp</t>
@@ -1030,6 +1030,9 @@
   </si>
   <si>
     <t>Explain why the sick needs to go to the health facility</t>
+  </si>
+  <si>
+    <t>li li</t>
   </si>
   <si>
     <t>summary_danger_signs2</t>
@@ -1417,8 +1420,7 @@
     <t>if(
     selected(${__any_danger}, 'no') and 
     ${diarrhea_last} &lt; 14 and
-    selected(${diarrhea_blood}, 'no') and
-    not(selected(${malaria_results}, 'positive'))
+    selected(${diarrhea_blood}, 'no')
     ,"yes", "no"
  )</t>
   </si>
@@ -1462,6 +1464,16 @@
     selected(${two_mo_referred}, 'yes')
     ,"yes", "no"
  )</t>
+  </si>
+  <si>
+    <t>__display_age</t>
+  </si>
+  <si>
+    <t>if(../../patient_age_in_days &lt; 31, 
+concat(../../patient_age_in_days, ' days old'),
+if(../../patient_age_in_months &lt; 12, 
+concat(../../patient_age_in_months, ' months old'), 
+concat(../../patient_age_in_years, ' years old')))</t>
   </si>
   <si>
     <t>list_name</t>
@@ -9030,7 +9042,7 @@
       <c r="J134" s="40"/>
       <c r="K134" s="45"/>
       <c r="L134" s="42" t="s">
-        <v>224</v>
+        <v>308</v>
       </c>
       <c r="M134" s="46"/>
       <c r="N134" s="46"/>
@@ -9065,10 +9077,10 @@
         <v>87</v>
       </c>
       <c r="B135" s="42" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="C135" s="42" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="D135" s="41"/>
       <c r="E135" s="40"/>
@@ -9114,10 +9126,10 @@
         <v>87</v>
       </c>
       <c r="B136" s="42" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C136" s="42" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="D136" s="41"/>
       <c r="E136" s="40"/>
@@ -9163,10 +9175,10 @@
         <v>87</v>
       </c>
       <c r="B137" s="42" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C137" s="42" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="D137" s="41"/>
       <c r="E137" s="40"/>
@@ -9212,10 +9224,10 @@
         <v>87</v>
       </c>
       <c r="B138" s="42" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C138" s="42" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="D138" s="41"/>
       <c r="E138" s="40"/>
@@ -9261,10 +9273,10 @@
         <v>87</v>
       </c>
       <c r="B139" s="42" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C139" s="42" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="D139" s="41"/>
       <c r="E139" s="40"/>
@@ -9353,7 +9365,7 @@
         <v>87</v>
       </c>
       <c r="B141" s="45" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="C141" s="45" t="s">
         <v>305</v>
@@ -9404,10 +9416,10 @@
         <v>87</v>
       </c>
       <c r="B142" s="42" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C142" s="42" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D142" s="46"/>
       <c r="E142" s="44"/>
@@ -9453,7 +9465,7 @@
         <v>87</v>
       </c>
       <c r="B143" s="45" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="C143" s="45" t="s">
         <v>305</v>
@@ -9504,7 +9516,7 @@
         <v>34</v>
       </c>
       <c r="B144" s="42" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="C144" s="40" t="s">
         <v>72</v>
@@ -9555,10 +9567,10 @@
         <v>87</v>
       </c>
       <c r="B145" s="42" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="C145" s="42" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="D145" s="46"/>
       <c r="E145" s="44"/>
@@ -9604,10 +9616,10 @@
         <v>87</v>
       </c>
       <c r="B146" s="42" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C146" s="53" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D146" s="41"/>
       <c r="E146" s="40"/>
@@ -9696,7 +9708,7 @@
         <v>34</v>
       </c>
       <c r="B148" s="42" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="C148" s="40" t="s">
         <v>72</v>
@@ -9747,10 +9759,10 @@
         <v>87</v>
       </c>
       <c r="B149" s="42" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="C149" s="52" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="D149" s="41"/>
       <c r="E149" s="40"/>
@@ -9796,10 +9808,10 @@
         <v>87</v>
       </c>
       <c r="B150" s="42" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C150" s="42" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D150" s="41"/>
       <c r="E150" s="40"/>
@@ -9845,10 +9857,10 @@
         <v>87</v>
       </c>
       <c r="B151" s="42" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="C151" s="42" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D151" s="41"/>
       <c r="E151" s="40"/>
@@ -9937,7 +9949,7 @@
         <v>34</v>
       </c>
       <c r="B153" s="42" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C153" s="40" t="s">
         <v>72</v>
@@ -9988,10 +10000,10 @@
         <v>87</v>
       </c>
       <c r="B154" s="42" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="C154" s="42" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D154" s="46"/>
       <c r="E154" s="44"/>
@@ -10037,10 +10049,10 @@
         <v>87</v>
       </c>
       <c r="B155" s="42" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C155" s="42" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="D155" s="46"/>
       <c r="E155" s="44"/>
@@ -10086,10 +10098,10 @@
         <v>87</v>
       </c>
       <c r="B156" s="42" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="C156" s="42" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D156" s="46"/>
       <c r="E156" s="44"/>
@@ -10178,7 +10190,7 @@
         <v>34</v>
       </c>
       <c r="B158" s="42" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C158" s="40" t="s">
         <v>72</v>
@@ -10229,10 +10241,10 @@
         <v>87</v>
       </c>
       <c r="B159" s="42" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C159" s="42" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="D159" s="41"/>
       <c r="E159" s="40"/>
@@ -10278,10 +10290,10 @@
         <v>87</v>
       </c>
       <c r="B160" s="42" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C160" s="42" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D160" s="41"/>
       <c r="E160" s="40"/>
@@ -10370,7 +10382,7 @@
         <v>34</v>
       </c>
       <c r="B162" s="42" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="C162" s="40" t="s">
         <v>72</v>
@@ -10421,10 +10433,10 @@
         <v>87</v>
       </c>
       <c r="B163" s="42" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C163" s="42" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="D163" s="41"/>
       <c r="E163" s="40"/>
@@ -10470,10 +10482,10 @@
         <v>87</v>
       </c>
       <c r="B164" s="42" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C164" s="42" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="D164" s="41"/>
       <c r="E164" s="40"/>
@@ -10562,10 +10574,10 @@
         <v>87</v>
       </c>
       <c r="B166" s="42" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="C166" s="42" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D166" s="41"/>
       <c r="E166" s="40"/>
@@ -10575,7 +10587,7 @@
       <c r="I166" s="41"/>
       <c r="J166" s="40"/>
       <c r="K166" s="42" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="L166" s="42" t="s">
         <v>224</v>
@@ -10613,10 +10625,10 @@
         <v>87</v>
       </c>
       <c r="B167" s="42" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C167" s="42" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="D167" s="41"/>
       <c r="E167" s="40"/>
@@ -10664,10 +10676,10 @@
         <v>87</v>
       </c>
       <c r="B168" s="42" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="C168" s="42" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D168" s="41"/>
       <c r="E168" s="40"/>
@@ -10717,7 +10729,7 @@
         <v>34</v>
       </c>
       <c r="B169" s="42" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="C169" s="40" t="s">
         <v>72</v>
@@ -10768,10 +10780,10 @@
         <v>87</v>
       </c>
       <c r="B170" s="42" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="C170" s="42" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D170" s="41"/>
       <c r="E170" s="40"/>
@@ -10817,10 +10829,10 @@
         <v>87</v>
       </c>
       <c r="B171" s="42" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C171" s="42" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D171" s="41"/>
       <c r="E171" s="40"/>
@@ -10911,7 +10923,7 @@
         <v>34</v>
       </c>
       <c r="B173" s="42" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="C173" s="40" t="s">
         <v>72</v>
@@ -10962,10 +10974,10 @@
         <v>87</v>
       </c>
       <c r="B174" s="42" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="C174" s="42" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D174" s="41"/>
       <c r="E174" s="40"/>
@@ -11011,10 +11023,10 @@
         <v>87</v>
       </c>
       <c r="B175" s="42" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="C175" s="42" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D175" s="41"/>
       <c r="E175" s="40"/>
@@ -11103,7 +11115,7 @@
         <v>34</v>
       </c>
       <c r="B177" s="42" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C177" s="40" t="s">
         <v>72</v>
@@ -11116,7 +11128,7 @@
       <c r="I177" s="41"/>
       <c r="J177" s="40"/>
       <c r="K177" s="42" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="L177" s="42" t="s">
         <v>38</v>
@@ -11154,10 +11166,10 @@
         <v>87</v>
       </c>
       <c r="B178" s="42" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="C178" s="42" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="D178" s="41"/>
       <c r="E178" s="40"/>
@@ -11203,10 +11215,10 @@
         <v>87</v>
       </c>
       <c r="B179" s="42" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C179" s="42" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D179" s="41"/>
       <c r="E179" s="40"/>
@@ -11295,7 +11307,7 @@
         <v>34</v>
       </c>
       <c r="B181" s="42" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="C181" s="40" t="s">
         <v>72</v>
@@ -11308,7 +11320,7 @@
       <c r="I181" s="41"/>
       <c r="J181" s="40"/>
       <c r="K181" s="42" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="L181" s="42" t="s">
         <v>38</v>
@@ -11346,10 +11358,10 @@
         <v>87</v>
       </c>
       <c r="B182" s="42" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="C182" s="42" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="D182" s="41"/>
       <c r="E182" s="40"/>
@@ -11395,10 +11407,10 @@
         <v>87</v>
       </c>
       <c r="B183" s="42" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C183" s="42" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D183" s="41"/>
       <c r="E183" s="40"/>
@@ -11444,10 +11456,10 @@
         <v>87</v>
       </c>
       <c r="B184" s="42" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="C184" s="42" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="D184" s="41"/>
       <c r="E184" s="40"/>
@@ -11493,10 +11505,10 @@
         <v>87</v>
       </c>
       <c r="B185" s="42" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="C185" s="42" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="D185" s="41"/>
       <c r="E185" s="40"/>
@@ -11542,10 +11554,10 @@
         <v>87</v>
       </c>
       <c r="B186" s="42" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="C186" s="42" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D186" s="41"/>
       <c r="E186" s="40"/>
@@ -11634,7 +11646,7 @@
         <v>34</v>
       </c>
       <c r="B188" s="42" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C188" s="40" t="s">
         <v>72</v>
@@ -11647,7 +11659,7 @@
       <c r="I188" s="41"/>
       <c r="J188" s="40"/>
       <c r="K188" s="42" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="L188" s="42" t="s">
         <v>38</v>
@@ -11685,10 +11697,10 @@
         <v>87</v>
       </c>
       <c r="B189" s="42" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C189" s="42" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="D189" s="41"/>
       <c r="E189" s="40"/>
@@ -11734,10 +11746,10 @@
         <v>87</v>
       </c>
       <c r="B190" s="42" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C190" s="42" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="D190" s="41"/>
       <c r="E190" s="40"/>
@@ -11826,10 +11838,10 @@
         <v>87</v>
       </c>
       <c r="B192" s="42" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="C192" s="42" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="D192" s="41"/>
       <c r="E192" s="40"/>
@@ -11877,7 +11889,7 @@
         <v>34</v>
       </c>
       <c r="B193" s="42" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="C193" s="40" t="s">
         <v>72</v>
@@ -11928,10 +11940,10 @@
         <v>87</v>
       </c>
       <c r="B194" s="42" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="C194" s="42" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D194" s="41"/>
       <c r="E194" s="40"/>
@@ -11977,10 +11989,10 @@
         <v>87</v>
       </c>
       <c r="B195" s="42" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="C195" s="42" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="D195" s="41"/>
       <c r="E195" s="40"/>
@@ -12026,10 +12038,10 @@
         <v>87</v>
       </c>
       <c r="B196" s="42" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="C196" s="42" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D196" s="41"/>
       <c r="E196" s="40"/>
@@ -12118,7 +12130,7 @@
         <v>34</v>
       </c>
       <c r="B198" s="42" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C198" s="40" t="s">
         <v>72</v>
@@ -12169,10 +12181,10 @@
         <v>87</v>
       </c>
       <c r="B199" s="42" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="C199" s="42" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="D199" s="46"/>
       <c r="E199" s="44"/>
@@ -12216,10 +12228,10 @@
         <v>87</v>
       </c>
       <c r="B200" s="42" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="C200" s="42" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="D200" s="46"/>
       <c r="E200" s="44"/>
@@ -12263,10 +12275,10 @@
         <v>87</v>
       </c>
       <c r="B201" s="42" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="C201" s="42" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="D201" s="46"/>
       <c r="E201" s="44"/>
@@ -12354,7 +12366,7 @@
       </c>
       <c r="B203" s="44"/>
       <c r="C203" s="45" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="D203" s="46"/>
       <c r="E203" s="44"/>
@@ -12365,7 +12377,7 @@
       <c r="J203" s="44"/>
       <c r="K203" s="44"/>
       <c r="L203" s="45" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="M203" s="46"/>
       <c r="N203" s="46"/>
@@ -12401,7 +12413,7 @@
       </c>
       <c r="B204" s="40"/>
       <c r="C204" s="42" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="D204" s="41"/>
       <c r="E204" s="40"/>
@@ -12570,7 +12582,7 @@
         <v>34</v>
       </c>
       <c r="B208" s="54" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="C208" s="55" t="s">
         <v>72</v>
@@ -12621,7 +12633,7 @@
         <v>70</v>
       </c>
       <c r="B209" s="57" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="C209" s="55" t="s">
         <v>72</v>
@@ -12644,7 +12656,7 @@
       <c r="S209" s="56"/>
       <c r="T209" s="56"/>
       <c r="U209" s="58" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="V209" s="56"/>
       <c r="W209" s="56"/>
@@ -12659,7 +12671,7 @@
       <c r="AF209" s="55"/>
       <c r="AG209" s="55"/>
       <c r="AH209" s="59" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="AI209" s="60"/>
       <c r="AJ209" s="55"/>
@@ -12672,7 +12684,7 @@
         <v>70</v>
       </c>
       <c r="B210" s="57" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="C210" s="55" t="s">
         <v>72</v>
@@ -12695,7 +12707,7 @@
       <c r="S210" s="56"/>
       <c r="T210" s="56"/>
       <c r="U210" s="58" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="V210" s="56"/>
       <c r="W210" s="56"/>
@@ -12721,7 +12733,7 @@
         <v>70</v>
       </c>
       <c r="B211" s="57" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C211" s="55" t="s">
         <v>72</v>
@@ -12744,7 +12756,7 @@
       <c r="S211" s="56"/>
       <c r="T211" s="56"/>
       <c r="U211" s="58" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="V211" s="56"/>
       <c r="W211" s="56"/>
@@ -12770,7 +12782,7 @@
         <v>70</v>
       </c>
       <c r="B212" s="57" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C212" s="55" t="s">
         <v>72</v>
@@ -12793,7 +12805,7 @@
       <c r="S212" s="56"/>
       <c r="T212" s="56"/>
       <c r="U212" s="58" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="V212" s="56"/>
       <c r="W212" s="56"/>
@@ -12819,7 +12831,7 @@
         <v>70</v>
       </c>
       <c r="B213" s="57" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="C213" s="55" t="s">
         <v>72</v>
@@ -12842,7 +12854,7 @@
       <c r="S213" s="56"/>
       <c r="T213" s="56"/>
       <c r="U213" s="58" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="V213" s="56"/>
       <c r="W213" s="56"/>
@@ -12868,7 +12880,7 @@
         <v>70</v>
       </c>
       <c r="B214" s="57" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C214" s="55" t="s">
         <v>72</v>
@@ -12891,7 +12903,7 @@
       <c r="S214" s="56"/>
       <c r="T214" s="56"/>
       <c r="U214" s="58" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="V214" s="56"/>
       <c r="W214" s="56"/>
@@ -12917,7 +12929,7 @@
         <v>70</v>
       </c>
       <c r="B215" s="62" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="C215" s="55" t="s">
         <v>72</v>
@@ -12940,7 +12952,7 @@
       <c r="S215" s="56"/>
       <c r="T215" s="56"/>
       <c r="U215" s="58" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="V215" s="56"/>
       <c r="W215" s="56"/>
@@ -12966,7 +12978,7 @@
         <v>70</v>
       </c>
       <c r="B216" s="62" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="C216" s="55" t="s">
         <v>72</v>
@@ -12989,7 +13001,7 @@
       <c r="S216" s="56"/>
       <c r="T216" s="56"/>
       <c r="U216" s="58" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="V216" s="56"/>
       <c r="W216" s="56"/>
@@ -13015,7 +13027,7 @@
         <v>70</v>
       </c>
       <c r="B217" s="62" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C217" s="55" t="s">
         <v>72</v>
@@ -13038,7 +13050,7 @@
       <c r="S217" s="56"/>
       <c r="T217" s="56"/>
       <c r="U217" s="58" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="V217" s="56"/>
       <c r="W217" s="56"/>
@@ -13064,7 +13076,7 @@
         <v>70</v>
       </c>
       <c r="B218" s="62" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C218" s="55" t="s">
         <v>72</v>
@@ -13087,7 +13099,7 @@
       <c r="S218" s="56"/>
       <c r="T218" s="56"/>
       <c r="U218" s="58" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="V218" s="56"/>
       <c r="W218" s="56"/>
@@ -13113,7 +13125,7 @@
         <v>70</v>
       </c>
       <c r="B219" s="62" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="C219" s="55" t="s">
         <v>72</v>
@@ -13136,7 +13148,7 @@
       <c r="S219" s="56"/>
       <c r="T219" s="56"/>
       <c r="U219" s="58" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="V219" s="56"/>
       <c r="W219" s="56"/>
@@ -13162,7 +13174,7 @@
         <v>70</v>
       </c>
       <c r="B220" s="62" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C220" s="55" t="s">
         <v>72</v>
@@ -13185,7 +13197,7 @@
       <c r="S220" s="56"/>
       <c r="T220" s="56"/>
       <c r="U220" s="58" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="V220" s="56"/>
       <c r="W220" s="56"/>
@@ -13207,11 +13219,15 @@
       <c r="AM220" s="19"/>
     </row>
     <row r="221" ht="15.75" customHeight="1">
-      <c r="A221" s="61" t="s">
-        <v>69</v>
-      </c>
-      <c r="B221" s="61"/>
-      <c r="C221" s="55"/>
+      <c r="A221" s="62" t="s">
+        <v>70</v>
+      </c>
+      <c r="B221" s="62" t="s">
+        <v>418</v>
+      </c>
+      <c r="C221" s="58" t="s">
+        <v>72</v>
+      </c>
       <c r="D221" s="56"/>
       <c r="E221" s="55"/>
       <c r="F221" s="55"/>
@@ -13229,7 +13245,9 @@
       <c r="R221" s="56"/>
       <c r="S221" s="56"/>
       <c r="T221" s="56"/>
-      <c r="U221" s="56"/>
+      <c r="U221" s="58" t="s">
+        <v>419</v>
+      </c>
       <c r="V221" s="56"/>
       <c r="W221" s="56"/>
       <c r="X221" s="56"/>
@@ -13250,41 +13268,44 @@
       <c r="AM221" s="19"/>
     </row>
     <row r="222" ht="15.75" customHeight="1">
-      <c r="A222" s="18"/>
-      <c r="B222" s="18"/>
-      <c r="C222" s="18"/>
-      <c r="D222" s="10"/>
-      <c r="E222" s="18"/>
-      <c r="F222" s="18"/>
-      <c r="G222" s="10"/>
-      <c r="H222" s="10"/>
-      <c r="I222" s="10"/>
-      <c r="J222" s="10"/>
-      <c r="K222" s="18"/>
-      <c r="L222" s="18"/>
-      <c r="M222" s="10"/>
-      <c r="N222" s="10"/>
-      <c r="O222" s="10"/>
-      <c r="P222" s="10"/>
-      <c r="Q222" s="10"/>
-      <c r="R222" s="10"/>
-      <c r="S222" s="10"/>
-      <c r="T222" s="10"/>
-      <c r="V222" s="10"/>
-      <c r="W222" s="10"/>
-      <c r="X222" s="10"/>
-      <c r="Y222" s="10"/>
-      <c r="Z222" s="10"/>
-      <c r="AA222" s="10"/>
-      <c r="AB222" s="10"/>
-      <c r="AC222" s="10"/>
-      <c r="AD222" s="10"/>
-      <c r="AE222" s="10"/>
-      <c r="AF222" s="19"/>
-      <c r="AG222" s="19"/>
-      <c r="AH222" s="19"/>
-      <c r="AI222" s="19"/>
-      <c r="AJ222" s="19"/>
+      <c r="A222" s="61" t="s">
+        <v>69</v>
+      </c>
+      <c r="B222" s="61"/>
+      <c r="C222" s="55"/>
+      <c r="D222" s="56"/>
+      <c r="E222" s="55"/>
+      <c r="F222" s="55"/>
+      <c r="G222" s="56"/>
+      <c r="H222" s="56"/>
+      <c r="I222" s="56"/>
+      <c r="J222" s="56"/>
+      <c r="K222" s="55"/>
+      <c r="L222" s="55"/>
+      <c r="M222" s="56"/>
+      <c r="N222" s="56"/>
+      <c r="O222" s="56"/>
+      <c r="P222" s="56"/>
+      <c r="Q222" s="56"/>
+      <c r="R222" s="56"/>
+      <c r="S222" s="56"/>
+      <c r="T222" s="56"/>
+      <c r="U222" s="56"/>
+      <c r="V222" s="56"/>
+      <c r="W222" s="56"/>
+      <c r="X222" s="56"/>
+      <c r="Y222" s="56"/>
+      <c r="Z222" s="56"/>
+      <c r="AA222" s="56"/>
+      <c r="AB222" s="56"/>
+      <c r="AC222" s="56"/>
+      <c r="AD222" s="56"/>
+      <c r="AE222" s="56"/>
+      <c r="AF222" s="55"/>
+      <c r="AG222" s="55"/>
+      <c r="AH222" s="55"/>
+      <c r="AI222" s="55"/>
+      <c r="AJ222" s="55"/>
       <c r="AK222" s="19"/>
       <c r="AL222" s="19"/>
       <c r="AM222" s="19"/>
@@ -13310,7 +13331,6 @@
       <c r="R223" s="10"/>
       <c r="S223" s="10"/>
       <c r="T223" s="10"/>
-      <c r="U223" s="10"/>
       <c r="V223" s="10"/>
       <c r="W223" s="10"/>
       <c r="X223" s="10"/>
@@ -13659,39 +13679,39 @@
       <c r="AM231" s="19"/>
     </row>
     <row r="232" ht="15.75" customHeight="1">
-      <c r="A232" s="63"/>
-      <c r="B232" s="63"/>
-      <c r="C232" s="63"/>
-      <c r="D232" s="64"/>
-      <c r="E232" s="63"/>
-      <c r="F232" s="63"/>
-      <c r="G232" s="64"/>
-      <c r="H232" s="64"/>
-      <c r="I232" s="64"/>
-      <c r="J232" s="64"/>
-      <c r="K232" s="63"/>
-      <c r="L232" s="63"/>
-      <c r="M232" s="64"/>
-      <c r="N232" s="64"/>
-      <c r="O232" s="64"/>
-      <c r="P232" s="64"/>
-      <c r="Q232" s="64"/>
-      <c r="R232" s="64"/>
-      <c r="S232" s="64"/>
-      <c r="T232" s="64"/>
-      <c r="U232" s="64"/>
-      <c r="V232" s="64"/>
-      <c r="W232" s="64"/>
-      <c r="X232" s="64"/>
-      <c r="Y232" s="64"/>
-      <c r="Z232" s="64"/>
-      <c r="AA232" s="64"/>
-      <c r="AB232" s="64"/>
-      <c r="AC232" s="64"/>
-      <c r="AD232" s="64"/>
-      <c r="AE232" s="64"/>
-      <c r="AF232" s="65"/>
-      <c r="AG232" s="65"/>
+      <c r="A232" s="18"/>
+      <c r="B232" s="18"/>
+      <c r="C232" s="18"/>
+      <c r="D232" s="10"/>
+      <c r="E232" s="18"/>
+      <c r="F232" s="18"/>
+      <c r="G232" s="10"/>
+      <c r="H232" s="10"/>
+      <c r="I232" s="10"/>
+      <c r="J232" s="10"/>
+      <c r="K232" s="18"/>
+      <c r="L232" s="18"/>
+      <c r="M232" s="10"/>
+      <c r="N232" s="10"/>
+      <c r="O232" s="10"/>
+      <c r="P232" s="10"/>
+      <c r="Q232" s="10"/>
+      <c r="R232" s="10"/>
+      <c r="S232" s="10"/>
+      <c r="T232" s="10"/>
+      <c r="U232" s="10"/>
+      <c r="V232" s="10"/>
+      <c r="W232" s="10"/>
+      <c r="X232" s="10"/>
+      <c r="Y232" s="10"/>
+      <c r="Z232" s="10"/>
+      <c r="AA232" s="10"/>
+      <c r="AB232" s="10"/>
+      <c r="AC232" s="10"/>
+      <c r="AD232" s="10"/>
+      <c r="AE232" s="10"/>
+      <c r="AF232" s="19"/>
+      <c r="AG232" s="19"/>
       <c r="AH232" s="19"/>
       <c r="AI232" s="19"/>
       <c r="AJ232" s="19"/>
@@ -13792,7 +13812,7 @@
       <c r="H235" s="64"/>
       <c r="I235" s="64"/>
       <c r="J235" s="64"/>
-      <c r="K235" s="64"/>
+      <c r="K235" s="63"/>
       <c r="L235" s="63"/>
       <c r="M235" s="64"/>
       <c r="N235" s="64"/>
@@ -13823,18 +13843,18 @@
       <c r="AM235" s="19"/>
     </row>
     <row r="236" ht="15.75" customHeight="1">
-      <c r="A236" s="66"/>
-      <c r="B236" s="66"/>
-      <c r="C236" s="66"/>
-      <c r="D236" s="67"/>
-      <c r="E236" s="66"/>
-      <c r="F236" s="66"/>
-      <c r="G236" s="67"/>
-      <c r="H236" s="67"/>
-      <c r="I236" s="67"/>
-      <c r="J236" s="67"/>
-      <c r="K236" s="67"/>
-      <c r="L236" s="66"/>
+      <c r="A236" s="63"/>
+      <c r="B236" s="63"/>
+      <c r="C236" s="63"/>
+      <c r="D236" s="64"/>
+      <c r="E236" s="63"/>
+      <c r="F236" s="63"/>
+      <c r="G236" s="64"/>
+      <c r="H236" s="64"/>
+      <c r="I236" s="64"/>
+      <c r="J236" s="64"/>
+      <c r="K236" s="64"/>
+      <c r="L236" s="63"/>
       <c r="M236" s="64"/>
       <c r="N236" s="64"/>
       <c r="O236" s="64"/>
@@ -13864,18 +13884,18 @@
       <c r="AM236" s="19"/>
     </row>
     <row r="237" ht="15.75" customHeight="1">
-      <c r="A237" s="63"/>
-      <c r="B237" s="63"/>
-      <c r="C237" s="63"/>
-      <c r="D237" s="64"/>
-      <c r="E237" s="63"/>
-      <c r="F237" s="63"/>
-      <c r="G237" s="64"/>
-      <c r="H237" s="64"/>
-      <c r="I237" s="64"/>
-      <c r="J237" s="64"/>
-      <c r="K237" s="63"/>
-      <c r="L237" s="63"/>
+      <c r="A237" s="66"/>
+      <c r="B237" s="66"/>
+      <c r="C237" s="66"/>
+      <c r="D237" s="67"/>
+      <c r="E237" s="66"/>
+      <c r="F237" s="66"/>
+      <c r="G237" s="67"/>
+      <c r="H237" s="67"/>
+      <c r="I237" s="67"/>
+      <c r="J237" s="67"/>
+      <c r="K237" s="67"/>
+      <c r="L237" s="66"/>
       <c r="M237" s="64"/>
       <c r="N237" s="64"/>
       <c r="O237" s="64"/>
@@ -14325,7 +14345,7 @@
       <c r="H248" s="64"/>
       <c r="I248" s="64"/>
       <c r="J248" s="64"/>
-      <c r="K248" s="64"/>
+      <c r="K248" s="63"/>
       <c r="L248" s="63"/>
       <c r="M248" s="64"/>
       <c r="N248" s="64"/>
@@ -14356,18 +14376,18 @@
       <c r="AM248" s="19"/>
     </row>
     <row r="249" ht="15.75" customHeight="1">
-      <c r="A249" s="66"/>
-      <c r="B249" s="68"/>
-      <c r="C249" s="66"/>
-      <c r="D249" s="67"/>
-      <c r="E249" s="66"/>
-      <c r="F249" s="66"/>
-      <c r="G249" s="67"/>
-      <c r="H249" s="67"/>
-      <c r="I249" s="67"/>
-      <c r="J249" s="67"/>
-      <c r="K249" s="67"/>
-      <c r="L249" s="66"/>
+      <c r="A249" s="63"/>
+      <c r="B249" s="63"/>
+      <c r="C249" s="63"/>
+      <c r="D249" s="64"/>
+      <c r="E249" s="63"/>
+      <c r="F249" s="63"/>
+      <c r="G249" s="64"/>
+      <c r="H249" s="64"/>
+      <c r="I249" s="64"/>
+      <c r="J249" s="64"/>
+      <c r="K249" s="64"/>
+      <c r="L249" s="63"/>
       <c r="M249" s="64"/>
       <c r="N249" s="64"/>
       <c r="O249" s="64"/>
@@ -14397,18 +14417,18 @@
       <c r="AM249" s="19"/>
     </row>
     <row r="250" ht="15.75" customHeight="1">
-      <c r="A250" s="63"/>
-      <c r="B250" s="63"/>
-      <c r="C250" s="63"/>
-      <c r="D250" s="64"/>
-      <c r="E250" s="63"/>
-      <c r="F250" s="63"/>
-      <c r="G250" s="64"/>
-      <c r="H250" s="64"/>
-      <c r="I250" s="64"/>
-      <c r="J250" s="64"/>
-      <c r="K250" s="63"/>
-      <c r="L250" s="63"/>
+      <c r="A250" s="66"/>
+      <c r="B250" s="68"/>
+      <c r="C250" s="66"/>
+      <c r="D250" s="67"/>
+      <c r="E250" s="66"/>
+      <c r="F250" s="66"/>
+      <c r="G250" s="67"/>
+      <c r="H250" s="67"/>
+      <c r="I250" s="67"/>
+      <c r="J250" s="67"/>
+      <c r="K250" s="67"/>
+      <c r="L250" s="66"/>
       <c r="M250" s="64"/>
       <c r="N250" s="64"/>
       <c r="O250" s="64"/>
@@ -14601,7 +14621,7 @@
       <c r="AL254" s="19"/>
       <c r="AM254" s="19"/>
     </row>
-    <row r="255">
+    <row r="255" ht="15.75" customHeight="1">
       <c r="A255" s="63"/>
       <c r="B255" s="63"/>
       <c r="C255" s="63"/>
@@ -14612,7 +14632,7 @@
       <c r="H255" s="64"/>
       <c r="I255" s="64"/>
       <c r="J255" s="64"/>
-      <c r="K255" s="64"/>
+      <c r="K255" s="63"/>
       <c r="L255" s="63"/>
       <c r="M255" s="64"/>
       <c r="N255" s="64"/>
@@ -14622,7 +14642,7 @@
       <c r="R255" s="64"/>
       <c r="S255" s="64"/>
       <c r="T255" s="64"/>
-      <c r="U255" s="63"/>
+      <c r="U255" s="64"/>
       <c r="V255" s="64"/>
       <c r="W255" s="64"/>
       <c r="X255" s="64"/>
@@ -14642,7 +14662,7 @@
       <c r="AL255" s="19"/>
       <c r="AM255" s="19"/>
     </row>
-    <row r="256" ht="15.75" customHeight="1">
+    <row r="256">
       <c r="A256" s="63"/>
       <c r="B256" s="63"/>
       <c r="C256" s="63"/>
@@ -14729,8 +14749,8 @@
       <c r="B258" s="63"/>
       <c r="C258" s="63"/>
       <c r="D258" s="64"/>
-      <c r="E258" s="64"/>
-      <c r="F258" s="64"/>
+      <c r="E258" s="63"/>
+      <c r="F258" s="63"/>
       <c r="G258" s="64"/>
       <c r="H258" s="64"/>
       <c r="I258" s="64"/>
@@ -14756,17 +14776,19 @@
       <c r="AC258" s="64"/>
       <c r="AD258" s="64"/>
       <c r="AE258" s="64"/>
-      <c r="AH258" s="69"/>
-      <c r="AI258" s="69"/>
-      <c r="AJ258" s="69"/>
-      <c r="AK258" s="69"/>
-      <c r="AL258" s="69"/>
-      <c r="AM258" s="69"/>
+      <c r="AF258" s="65"/>
+      <c r="AG258" s="65"/>
+      <c r="AH258" s="19"/>
+      <c r="AI258" s="19"/>
+      <c r="AJ258" s="19"/>
+      <c r="AK258" s="19"/>
+      <c r="AL258" s="19"/>
+      <c r="AM258" s="19"/>
     </row>
     <row r="259" ht="15.75" customHeight="1">
       <c r="A259" s="63"/>
       <c r="B259" s="63"/>
-      <c r="C259" s="64"/>
+      <c r="C259" s="63"/>
       <c r="D259" s="64"/>
       <c r="E259" s="64"/>
       <c r="F259" s="64"/>
@@ -14922,15 +14944,15 @@
     <row r="263" ht="15.75" customHeight="1">
       <c r="A263" s="63"/>
       <c r="B263" s="63"/>
-      <c r="C263" s="63"/>
+      <c r="C263" s="64"/>
       <c r="D263" s="64"/>
-      <c r="E263" s="63"/>
+      <c r="E263" s="64"/>
       <c r="F263" s="64"/>
       <c r="G263" s="64"/>
       <c r="H263" s="64"/>
       <c r="I263" s="64"/>
       <c r="J263" s="64"/>
-      <c r="K263" s="63"/>
+      <c r="K263" s="64"/>
       <c r="L263" s="63"/>
       <c r="M263" s="64"/>
       <c r="N263" s="64"/>
@@ -14940,7 +14962,7 @@
       <c r="R263" s="64"/>
       <c r="S263" s="64"/>
       <c r="T263" s="64"/>
-      <c r="U263" s="64"/>
+      <c r="U263" s="63"/>
       <c r="V263" s="64"/>
       <c r="W263" s="64"/>
       <c r="X263" s="64"/>
@@ -14951,12 +14973,12 @@
       <c r="AC263" s="64"/>
       <c r="AD263" s="64"/>
       <c r="AE263" s="64"/>
-      <c r="AH263" s="70"/>
-      <c r="AI263" s="70"/>
-      <c r="AJ263" s="70"/>
-      <c r="AK263" s="70"/>
-      <c r="AL263" s="70"/>
-      <c r="AM263" s="70"/>
+      <c r="AH263" s="69"/>
+      <c r="AI263" s="69"/>
+      <c r="AJ263" s="69"/>
+      <c r="AK263" s="69"/>
+      <c r="AL263" s="69"/>
+      <c r="AM263" s="69"/>
     </row>
     <row r="264" ht="15.75" customHeight="1">
       <c r="A264" s="63"/>
@@ -14964,13 +14986,13 @@
       <c r="C264" s="63"/>
       <c r="D264" s="64"/>
       <c r="E264" s="63"/>
-      <c r="F264" s="63"/>
+      <c r="F264" s="64"/>
       <c r="G264" s="64"/>
       <c r="H264" s="64"/>
       <c r="I264" s="64"/>
       <c r="J264" s="64"/>
-      <c r="K264" s="64"/>
-      <c r="L264" s="64"/>
+      <c r="K264" s="63"/>
+      <c r="L264" s="63"/>
       <c r="M264" s="64"/>
       <c r="N264" s="64"/>
       <c r="O264" s="64"/>
@@ -14990,22 +15012,20 @@
       <c r="AC264" s="64"/>
       <c r="AD264" s="64"/>
       <c r="AE264" s="64"/>
-      <c r="AF264" s="65"/>
-      <c r="AG264" s="65"/>
-      <c r="AH264" s="19"/>
-      <c r="AI264" s="19"/>
-      <c r="AJ264" s="19"/>
-      <c r="AK264" s="19"/>
-      <c r="AL264" s="19"/>
-      <c r="AM264" s="19"/>
+      <c r="AH264" s="70"/>
+      <c r="AI264" s="70"/>
+      <c r="AJ264" s="70"/>
+      <c r="AK264" s="70"/>
+      <c r="AL264" s="70"/>
+      <c r="AM264" s="70"/>
     </row>
     <row r="265" ht="15.75" customHeight="1">
-      <c r="A265" s="64"/>
-      <c r="B265" s="64"/>
-      <c r="C265" s="64"/>
+      <c r="A265" s="63"/>
+      <c r="B265" s="63"/>
+      <c r="C265" s="63"/>
       <c r="D265" s="64"/>
-      <c r="E265" s="64"/>
-      <c r="F265" s="64"/>
+      <c r="E265" s="63"/>
+      <c r="F265" s="63"/>
       <c r="G265" s="64"/>
       <c r="H265" s="64"/>
       <c r="I265" s="64"/>
@@ -15031,6 +15051,8 @@
       <c r="AC265" s="64"/>
       <c r="AD265" s="64"/>
       <c r="AE265" s="64"/>
+      <c r="AF265" s="65"/>
+      <c r="AG265" s="65"/>
       <c r="AH265" s="19"/>
       <c r="AI265" s="19"/>
       <c r="AJ265" s="19"/>
@@ -15039,18 +15061,18 @@
       <c r="AM265" s="19"/>
     </row>
     <row r="266" ht="15.75" customHeight="1">
-      <c r="A266" s="63"/>
-      <c r="B266" s="63"/>
-      <c r="C266" s="63"/>
+      <c r="A266" s="64"/>
+      <c r="B266" s="64"/>
+      <c r="C266" s="64"/>
       <c r="D266" s="64"/>
-      <c r="E266" s="63"/>
-      <c r="F266" s="63"/>
+      <c r="E266" s="64"/>
+      <c r="F266" s="64"/>
       <c r="G266" s="64"/>
       <c r="H266" s="64"/>
       <c r="I266" s="64"/>
       <c r="J266" s="64"/>
       <c r="K266" s="64"/>
-      <c r="L266" s="63"/>
+      <c r="L266" s="64"/>
       <c r="M266" s="64"/>
       <c r="N266" s="64"/>
       <c r="O266" s="64"/>
@@ -15070,7 +15092,6 @@
       <c r="AC266" s="64"/>
       <c r="AD266" s="64"/>
       <c r="AE266" s="64"/>
-      <c r="AG266" s="65"/>
       <c r="AH266" s="19"/>
       <c r="AI266" s="19"/>
       <c r="AJ266" s="19"/>
@@ -15080,7 +15101,7 @@
     </row>
     <row r="267" ht="15.75" customHeight="1">
       <c r="A267" s="63"/>
-      <c r="B267" s="71"/>
+      <c r="B267" s="63"/>
       <c r="C267" s="63"/>
       <c r="D267" s="64"/>
       <c r="E267" s="63"/>
@@ -15090,7 +15111,7 @@
       <c r="I267" s="64"/>
       <c r="J267" s="64"/>
       <c r="K267" s="64"/>
-      <c r="L267" s="64"/>
+      <c r="L267" s="63"/>
       <c r="M267" s="64"/>
       <c r="N267" s="64"/>
       <c r="O267" s="64"/>
@@ -15099,7 +15120,7 @@
       <c r="R267" s="64"/>
       <c r="S267" s="64"/>
       <c r="T267" s="64"/>
-      <c r="U267" s="63"/>
+      <c r="U267" s="64"/>
       <c r="V267" s="64"/>
       <c r="W267" s="64"/>
       <c r="X267" s="64"/>
@@ -15110,9 +15131,8 @@
       <c r="AC267" s="64"/>
       <c r="AD267" s="64"/>
       <c r="AE267" s="64"/>
-      <c r="AF267" s="65"/>
       <c r="AG267" s="65"/>
-      <c r="AH267" s="72"/>
+      <c r="AH267" s="19"/>
       <c r="AI267" s="19"/>
       <c r="AJ267" s="19"/>
       <c r="AK267" s="19"/>
@@ -16288,7 +16308,7 @@
       <c r="R296" s="64"/>
       <c r="S296" s="64"/>
       <c r="T296" s="64"/>
-      <c r="U296" s="71"/>
+      <c r="U296" s="63"/>
       <c r="V296" s="64"/>
       <c r="W296" s="64"/>
       <c r="X296" s="64"/>
@@ -16329,7 +16349,7 @@
       <c r="R297" s="64"/>
       <c r="S297" s="64"/>
       <c r="T297" s="64"/>
-      <c r="U297" s="63"/>
+      <c r="U297" s="71"/>
       <c r="V297" s="64"/>
       <c r="W297" s="64"/>
       <c r="X297" s="64"/>
@@ -16678,40 +16698,40 @@
       <c r="AM305" s="19"/>
     </row>
     <row r="306" ht="15.75" customHeight="1">
-      <c r="A306" s="73"/>
-      <c r="B306" s="73"/>
+      <c r="A306" s="63"/>
+      <c r="B306" s="71"/>
       <c r="C306" s="63"/>
-      <c r="D306" s="10"/>
-      <c r="E306" s="18"/>
-      <c r="F306" s="18"/>
-      <c r="G306" s="10"/>
-      <c r="H306" s="10"/>
-      <c r="I306" s="10"/>
-      <c r="J306" s="10"/>
-      <c r="K306" s="10"/>
-      <c r="L306" s="10"/>
-      <c r="M306" s="10"/>
-      <c r="N306" s="10"/>
-      <c r="O306" s="10"/>
-      <c r="P306" s="10"/>
-      <c r="Q306" s="10"/>
-      <c r="R306" s="10"/>
-      <c r="S306" s="10"/>
-      <c r="T306" s="10"/>
-      <c r="U306" s="18"/>
-      <c r="V306" s="10"/>
-      <c r="W306" s="10"/>
-      <c r="X306" s="10"/>
-      <c r="Y306" s="10"/>
-      <c r="Z306" s="10"/>
-      <c r="AA306" s="10"/>
-      <c r="AB306" s="10"/>
-      <c r="AC306" s="10"/>
-      <c r="AD306" s="10"/>
-      <c r="AE306" s="10"/>
-      <c r="AF306" s="19"/>
-      <c r="AG306" s="19"/>
-      <c r="AH306" s="19"/>
+      <c r="D306" s="64"/>
+      <c r="E306" s="63"/>
+      <c r="F306" s="63"/>
+      <c r="G306" s="64"/>
+      <c r="H306" s="64"/>
+      <c r="I306" s="64"/>
+      <c r="J306" s="64"/>
+      <c r="K306" s="64"/>
+      <c r="L306" s="64"/>
+      <c r="M306" s="64"/>
+      <c r="N306" s="64"/>
+      <c r="O306" s="64"/>
+      <c r="P306" s="64"/>
+      <c r="Q306" s="64"/>
+      <c r="R306" s="64"/>
+      <c r="S306" s="64"/>
+      <c r="T306" s="64"/>
+      <c r="U306" s="63"/>
+      <c r="V306" s="64"/>
+      <c r="W306" s="64"/>
+      <c r="X306" s="64"/>
+      <c r="Y306" s="64"/>
+      <c r="Z306" s="64"/>
+      <c r="AA306" s="64"/>
+      <c r="AB306" s="64"/>
+      <c r="AC306" s="64"/>
+      <c r="AD306" s="64"/>
+      <c r="AE306" s="64"/>
+      <c r="AF306" s="65"/>
+      <c r="AG306" s="65"/>
+      <c r="AH306" s="72"/>
       <c r="AI306" s="19"/>
       <c r="AJ306" s="19"/>
       <c r="AK306" s="19"/>
@@ -16719,39 +16739,39 @@
       <c r="AM306" s="19"/>
     </row>
     <row r="307" ht="15.75" customHeight="1">
-      <c r="A307" s="63"/>
-      <c r="B307" s="71"/>
+      <c r="A307" s="73"/>
+      <c r="B307" s="73"/>
       <c r="C307" s="63"/>
-      <c r="D307" s="64"/>
-      <c r="E307" s="63"/>
-      <c r="F307" s="63"/>
-      <c r="G307" s="64"/>
-      <c r="H307" s="64"/>
-      <c r="I307" s="64"/>
-      <c r="J307" s="64"/>
-      <c r="K307" s="64"/>
-      <c r="L307" s="64"/>
-      <c r="M307" s="64"/>
-      <c r="N307" s="64"/>
-      <c r="O307" s="64"/>
-      <c r="P307" s="64"/>
-      <c r="Q307" s="64"/>
-      <c r="R307" s="64"/>
-      <c r="S307" s="64"/>
-      <c r="T307" s="64"/>
-      <c r="U307" s="71"/>
-      <c r="V307" s="64"/>
-      <c r="W307" s="64"/>
-      <c r="X307" s="64"/>
-      <c r="Y307" s="64"/>
-      <c r="Z307" s="64"/>
-      <c r="AA307" s="64"/>
-      <c r="AB307" s="64"/>
-      <c r="AC307" s="64"/>
-      <c r="AD307" s="64"/>
-      <c r="AE307" s="64"/>
-      <c r="AF307" s="65"/>
-      <c r="AG307" s="65"/>
+      <c r="D307" s="10"/>
+      <c r="E307" s="18"/>
+      <c r="F307" s="18"/>
+      <c r="G307" s="10"/>
+      <c r="H307" s="10"/>
+      <c r="I307" s="10"/>
+      <c r="J307" s="10"/>
+      <c r="K307" s="10"/>
+      <c r="L307" s="10"/>
+      <c r="M307" s="10"/>
+      <c r="N307" s="10"/>
+      <c r="O307" s="10"/>
+      <c r="P307" s="10"/>
+      <c r="Q307" s="10"/>
+      <c r="R307" s="10"/>
+      <c r="S307" s="10"/>
+      <c r="T307" s="10"/>
+      <c r="U307" s="18"/>
+      <c r="V307" s="10"/>
+      <c r="W307" s="10"/>
+      <c r="X307" s="10"/>
+      <c r="Y307" s="10"/>
+      <c r="Z307" s="10"/>
+      <c r="AA307" s="10"/>
+      <c r="AB307" s="10"/>
+      <c r="AC307" s="10"/>
+      <c r="AD307" s="10"/>
+      <c r="AE307" s="10"/>
+      <c r="AF307" s="19"/>
+      <c r="AG307" s="19"/>
       <c r="AH307" s="19"/>
       <c r="AI307" s="19"/>
       <c r="AJ307" s="19"/>
@@ -16834,7 +16854,7 @@
       <c r="AE309" s="64"/>
       <c r="AF309" s="65"/>
       <c r="AG309" s="65"/>
-      <c r="AH309" s="72"/>
+      <c r="AH309" s="19"/>
       <c r="AI309" s="19"/>
       <c r="AJ309" s="19"/>
       <c r="AK309" s="19"/>
@@ -16875,7 +16895,7 @@
       <c r="AE310" s="64"/>
       <c r="AF310" s="65"/>
       <c r="AG310" s="65"/>
-      <c r="AH310" s="19"/>
+      <c r="AH310" s="72"/>
       <c r="AI310" s="19"/>
       <c r="AJ310" s="19"/>
       <c r="AK310" s="19"/>
@@ -16924,39 +16944,39 @@
       <c r="AM311" s="19"/>
     </row>
     <row r="312" ht="15.75" customHeight="1">
-      <c r="A312" s="73"/>
-      <c r="B312" s="73"/>
-      <c r="C312" s="18"/>
-      <c r="D312" s="10"/>
-      <c r="E312" s="18"/>
-      <c r="F312" s="18"/>
-      <c r="G312" s="10"/>
-      <c r="H312" s="10"/>
-      <c r="I312" s="10"/>
-      <c r="J312" s="10"/>
-      <c r="K312" s="10"/>
-      <c r="L312" s="10"/>
-      <c r="M312" s="10"/>
-      <c r="N312" s="10"/>
-      <c r="O312" s="10"/>
-      <c r="P312" s="10"/>
-      <c r="Q312" s="10"/>
-      <c r="R312" s="10"/>
-      <c r="S312" s="10"/>
-      <c r="T312" s="10"/>
-      <c r="U312" s="10"/>
-      <c r="V312" s="10"/>
-      <c r="W312" s="10"/>
-      <c r="X312" s="10"/>
-      <c r="Y312" s="10"/>
-      <c r="Z312" s="10"/>
-      <c r="AA312" s="10"/>
-      <c r="AB312" s="10"/>
-      <c r="AC312" s="10"/>
-      <c r="AD312" s="10"/>
-      <c r="AE312" s="10"/>
-      <c r="AF312" s="19"/>
-      <c r="AG312" s="19"/>
+      <c r="A312" s="63"/>
+      <c r="B312" s="71"/>
+      <c r="C312" s="63"/>
+      <c r="D312" s="64"/>
+      <c r="E312" s="63"/>
+      <c r="F312" s="63"/>
+      <c r="G312" s="64"/>
+      <c r="H312" s="64"/>
+      <c r="I312" s="64"/>
+      <c r="J312" s="64"/>
+      <c r="K312" s="64"/>
+      <c r="L312" s="64"/>
+      <c r="M312" s="64"/>
+      <c r="N312" s="64"/>
+      <c r="O312" s="64"/>
+      <c r="P312" s="64"/>
+      <c r="Q312" s="64"/>
+      <c r="R312" s="64"/>
+      <c r="S312" s="64"/>
+      <c r="T312" s="64"/>
+      <c r="U312" s="71"/>
+      <c r="V312" s="64"/>
+      <c r="W312" s="64"/>
+      <c r="X312" s="64"/>
+      <c r="Y312" s="64"/>
+      <c r="Z312" s="64"/>
+      <c r="AA312" s="64"/>
+      <c r="AB312" s="64"/>
+      <c r="AC312" s="64"/>
+      <c r="AD312" s="64"/>
+      <c r="AE312" s="64"/>
+      <c r="AF312" s="65"/>
+      <c r="AG312" s="65"/>
       <c r="AH312" s="19"/>
       <c r="AI312" s="19"/>
       <c r="AJ312" s="19"/>
@@ -17415,9 +17435,50 @@
       <c r="AL323" s="19"/>
       <c r="AM323" s="19"/>
     </row>
+    <row r="324" ht="15.75" customHeight="1">
+      <c r="A324" s="73"/>
+      <c r="B324" s="73"/>
+      <c r="C324" s="18"/>
+      <c r="D324" s="10"/>
+      <c r="E324" s="18"/>
+      <c r="F324" s="18"/>
+      <c r="G324" s="10"/>
+      <c r="H324" s="10"/>
+      <c r="I324" s="10"/>
+      <c r="J324" s="10"/>
+      <c r="K324" s="10"/>
+      <c r="L324" s="10"/>
+      <c r="M324" s="10"/>
+      <c r="N324" s="10"/>
+      <c r="O324" s="10"/>
+      <c r="P324" s="10"/>
+      <c r="Q324" s="10"/>
+      <c r="R324" s="10"/>
+      <c r="S324" s="10"/>
+      <c r="T324" s="10"/>
+      <c r="U324" s="10"/>
+      <c r="V324" s="10"/>
+      <c r="W324" s="10"/>
+      <c r="X324" s="10"/>
+      <c r="Y324" s="10"/>
+      <c r="Z324" s="10"/>
+      <c r="AA324" s="10"/>
+      <c r="AB324" s="10"/>
+      <c r="AC324" s="10"/>
+      <c r="AD324" s="10"/>
+      <c r="AE324" s="10"/>
+      <c r="AF324" s="19"/>
+      <c r="AG324" s="19"/>
+      <c r="AH324" s="19"/>
+      <c r="AI324" s="19"/>
+      <c r="AJ324" s="19"/>
+      <c r="AK324" s="19"/>
+      <c r="AL324" s="19"/>
+      <c r="AM324" s="19"/>
+    </row>
   </sheetData>
   <dataValidations>
-    <dataValidation type="list" allowBlank="1" sqref="J2:J67 K68 J69:J76 K77 R168:R198 J78:J323">
+    <dataValidation type="list" allowBlank="1" sqref="J2:J67 K68 J69:J76 K77 R168:R198 J78:J324">
       <formula1>"yes,no"</formula1>
     </dataValidation>
   </dataValidations>
@@ -17445,7 +17506,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="74" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="B1" s="74" t="s">
         <v>1</v>
@@ -17487,13 +17548,13 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="72" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="B2" s="72" t="s">
         <v>85</v>
       </c>
       <c r="C2" s="72" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="D2" s="82"/>
       <c r="E2" s="82"/>
@@ -17517,13 +17578,13 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="72" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="B3" s="72" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="C3" s="72" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="D3" s="82"/>
       <c r="E3" s="82"/>
@@ -17571,13 +17632,13 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="72" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="B5" s="72" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="C5" s="72" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="D5" s="82"/>
       <c r="E5" s="82"/>
@@ -17601,13 +17662,13 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="72" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="B6" s="83" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="C6" s="83" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
       <c r="D6" s="82"/>
       <c r="E6" s="82"/>
@@ -17631,13 +17692,13 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="72" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="B7" s="72" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="C7" s="72" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
       <c r="D7" s="82"/>
       <c r="E7" s="82"/>
@@ -17661,13 +17722,13 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="72" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="B8" s="72" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="C8" s="72" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="D8" s="82"/>
       <c r="E8" s="82"/>
@@ -17715,13 +17776,13 @@
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="72" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="B10" s="83" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="C10" s="72" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="D10" s="82"/>
       <c r="E10" s="82"/>
@@ -17745,13 +17806,13 @@
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="72" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="B11" s="83" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="C11" s="72" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="D11" s="82"/>
       <c r="E11" s="82"/>
@@ -17799,13 +17860,13 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="84" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="B13" s="85" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="C13" s="84" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c r="D13" s="82"/>
       <c r="E13" s="82"/>
@@ -17829,13 +17890,13 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="84" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="B14" s="85" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="C14" s="84" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="D14" s="82"/>
       <c r="E14" s="82"/>
@@ -17859,13 +17920,13 @@
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="84" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="B15" s="85" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="C15" s="84" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
       <c r="D15" s="82"/>
       <c r="E15" s="82"/>
@@ -17913,13 +17974,13 @@
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="84" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="B17" s="84" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="C17" s="84" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="D17" s="82"/>
       <c r="E17" s="82"/>
@@ -17943,13 +18004,13 @@
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="84" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="B18" s="84" t="s">
         <v>85</v>
       </c>
       <c r="C18" s="84" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="D18" s="82"/>
       <c r="E18" s="82"/>
@@ -17997,13 +18058,13 @@
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="84" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="B20" s="82" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="C20" s="84" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="D20" s="82"/>
       <c r="E20" s="82"/>
@@ -18027,13 +18088,13 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="84" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="B21" s="82" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="C21" s="84" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="D21" s="82"/>
       <c r="E21" s="82"/>
@@ -18057,13 +18118,13 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="84" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="B22" s="82" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
       <c r="C22" s="84" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
       <c r="D22" s="82"/>
       <c r="E22" s="82"/>
@@ -18087,13 +18148,13 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="84" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="B23" s="84" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
       <c r="C23" s="84" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
       <c r="D23" s="82"/>
       <c r="E23" s="82"/>
@@ -18117,13 +18178,13 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="84" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="B24" s="85" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="C24" s="85" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="D24" s="82"/>
       <c r="E24" s="82"/>
@@ -18169,13 +18230,13 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="84" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
       <c r="B26" s="86" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="C26" s="84" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="D26" s="82"/>
       <c r="E26" s="82"/>
@@ -18199,13 +18260,13 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="84" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
       <c r="B27" s="84" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
       <c r="C27" s="84" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="D27" s="82"/>
       <c r="E27" s="82"/>
@@ -18229,13 +18290,13 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="84" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
       <c r="B28" s="84" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="C28" s="84" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="D28" s="82"/>
       <c r="E28" s="82"/>
@@ -18259,13 +18320,13 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="84" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
       <c r="B29" s="82" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="C29" s="86" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="D29" s="82"/>
       <c r="E29" s="82"/>
@@ -18289,13 +18350,13 @@
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="84" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
       <c r="B30" s="82" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="C30" s="84" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="D30" s="82"/>
       <c r="E30" s="82"/>
@@ -18319,13 +18380,13 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="84" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
       <c r="B31" s="82" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
       <c r="C31" s="84" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
       <c r="D31" s="82"/>
       <c r="E31" s="82"/>
@@ -18349,13 +18410,13 @@
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="84" t="s">
+        <v>460</v>
+      </c>
+      <c r="B32" s="84" t="s">
+        <v>456</v>
+      </c>
+      <c r="C32" s="84" t="s">
         <v>457</v>
-      </c>
-      <c r="B32" s="84" t="s">
-        <v>453</v>
-      </c>
-      <c r="C32" s="84" t="s">
-        <v>454</v>
       </c>
       <c r="D32" s="82"/>
       <c r="E32" s="82"/>
@@ -18379,13 +18440,13 @@
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="84" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
       <c r="B33" s="85" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="C33" s="85" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="D33" s="82"/>
       <c r="E33" s="82"/>
@@ -18433,24 +18494,24 @@
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="85" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
       <c r="B35" s="85" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
       <c r="C35" s="85" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="85" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="B36" s="85" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="C36" s="85" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1"/>
@@ -18463,7 +18524,7 @@
         <v>1.0</v>
       </c>
       <c r="C39" s="85" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
@@ -18474,7 +18535,7 @@
         <v>2.0</v>
       </c>
       <c r="C40" s="85" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
@@ -18485,7 +18546,7 @@
         <v>3.0</v>
       </c>
       <c r="C41" s="85" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
@@ -18496,7 +18557,7 @@
         <v>4.0</v>
       </c>
       <c r="C42" s="85" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
@@ -18507,7 +18568,7 @@
         <v>7.0</v>
       </c>
       <c r="C43" s="85" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
@@ -18518,7 +18579,7 @@
         <v>14.0</v>
       </c>
       <c r="C44" s="85" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
     </row>
     <row r="45" ht="15.75" customHeight="1">
@@ -18531,10 +18592,10 @@
         <v>138</v>
       </c>
       <c r="B46" s="85" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="C46" s="85" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
@@ -18542,10 +18603,10 @@
         <v>138</v>
       </c>
       <c r="B47" s="85" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="C47" s="85" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
     </row>
     <row r="48" ht="15.75" customHeight="1">
@@ -18553,10 +18614,10 @@
         <v>138</v>
       </c>
       <c r="B48" s="85" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="C48" s="85" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
     </row>
     <row r="49" ht="15.75" customHeight="1"/>
@@ -18565,10 +18626,10 @@
         <v>141</v>
       </c>
       <c r="B50" s="85" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="C50" s="85" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
     </row>
     <row r="51" ht="15.75" customHeight="1">
@@ -18576,10 +18637,10 @@
         <v>141</v>
       </c>
       <c r="B51" s="85" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="C51" s="85" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1"/>
@@ -18591,7 +18652,7 @@
         <v>1.0</v>
       </c>
       <c r="C53" s="85" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
@@ -18602,7 +18663,7 @@
         <v>2.0</v>
       </c>
       <c r="C54" s="85" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
     </row>
     <row r="55" ht="15.75" customHeight="1">
@@ -18613,7 +18674,7 @@
         <v>3.0</v>
       </c>
       <c r="C55" s="85" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
     </row>
     <row r="56" ht="15.75" customHeight="1">
@@ -18624,7 +18685,7 @@
         <v>4.0</v>
       </c>
       <c r="C56" s="85" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
     </row>
     <row r="57" ht="15.75" customHeight="1">
@@ -18635,7 +18696,7 @@
         <v>7.0</v>
       </c>
       <c r="C57" s="85" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
     </row>
     <row r="58" ht="15.75" customHeight="1">
@@ -18646,7 +18707,7 @@
         <v>14.0</v>
       </c>
       <c r="C58" s="85" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
     </row>
     <row r="59" ht="15.75" customHeight="1"/>
@@ -18658,7 +18719,7 @@
         <v>1.0</v>
       </c>
       <c r="C60" s="85" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
     </row>
     <row r="61" ht="15.75" customHeight="1">
@@ -18669,7 +18730,7 @@
         <v>2.0</v>
       </c>
       <c r="C61" s="85" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
     </row>
     <row r="62" ht="15.75" customHeight="1">
@@ -18680,7 +18741,7 @@
         <v>3.0</v>
       </c>
       <c r="C62" s="85" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
     </row>
     <row r="63" ht="15.75" customHeight="1">
@@ -18691,7 +18752,7 @@
         <v>4.0</v>
       </c>
       <c r="C63" s="85" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
     </row>
     <row r="64" ht="15.75" customHeight="1">
@@ -18702,7 +18763,7 @@
         <v>7.0</v>
       </c>
       <c r="C64" s="85" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
     </row>
     <row r="65" ht="15.75" customHeight="1">
@@ -18713,7 +18774,7 @@
         <v>14.0</v>
       </c>
       <c r="C65" s="85" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
     </row>
     <row r="66" ht="15.75" customHeight="1"/>
@@ -18722,10 +18783,10 @@
         <v>186</v>
       </c>
       <c r="B67" s="85" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
       <c r="C67" s="85" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
     </row>
     <row r="68" ht="15.75" customHeight="1">
@@ -18733,10 +18794,10 @@
         <v>186</v>
       </c>
       <c r="B68" s="85" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="C68" s="85" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
     </row>
     <row r="69" ht="15.75" customHeight="1"/>
@@ -18745,10 +18806,10 @@
         <v>195</v>
       </c>
       <c r="B70" s="85" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
       <c r="C70" s="85" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
     </row>
     <row r="71" ht="15.75" customHeight="1">
@@ -18756,10 +18817,10 @@
         <v>195</v>
       </c>
       <c r="B71" s="85" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
       <c r="C71" s="85" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
     </row>
     <row r="72" ht="15.75" customHeight="1">
@@ -18767,10 +18828,10 @@
         <v>195</v>
       </c>
       <c r="B72" s="85" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
       <c r="C72" s="89" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
     </row>
     <row r="73" ht="15.75" customHeight="1"/>
@@ -18823,25 +18884,25 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="74" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
       <c r="B1" s="74" t="s">
-        <v>497</v>
+        <v>500</v>
       </c>
       <c r="C1" s="74" t="s">
-        <v>498</v>
+        <v>501</v>
       </c>
       <c r="D1" s="74" t="s">
-        <v>499</v>
+        <v>502</v>
       </c>
       <c r="E1" s="74" t="s">
-        <v>500</v>
+        <v>503</v>
       </c>
       <c r="F1" s="74" t="s">
-        <v>501</v>
+        <v>504</v>
       </c>
       <c r="G1" s="90" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
       <c r="H1" s="74"/>
       <c r="I1" s="74"/>
@@ -18865,24 +18926,24 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="91" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="B2" s="91" t="s">
-        <v>504</v>
+        <v>507</v>
       </c>
       <c r="C2" s="92" t="str">
         <f>TEXT(NOW(), "yyyy-mm-dd_HH-MM")</f>
-        <v>2020-12-16_19-49</v>
+        <v>2021-01-04_15-49</v>
       </c>
       <c r="D2" s="93" t="s">
-        <v>505</v>
+        <v>508</v>
       </c>
       <c r="E2" s="93" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="F2" s="11"/>
       <c r="G2" s="94" t="s">
-        <v>506</v>
+        <v>509</v>
       </c>
       <c r="H2" s="11"/>
       <c r="I2" s="11"/>
@@ -19208,7 +19269,7 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="74" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="B1" s="74" t="s">
         <v>1</v>
@@ -19251,13 +19312,13 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="82" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="B2" s="82" t="s">
         <v>85</v>
       </c>
       <c r="C2" s="82" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="D2" s="82"/>
       <c r="E2" s="82"/>
@@ -19282,13 +19343,13 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="82" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="B3" s="82" t="s">
-        <v>420</v>
+        <v>423</v>
       </c>
       <c r="C3" s="82" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="D3" s="82"/>
       <c r="E3" s="82"/>
@@ -19338,13 +19399,13 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="82" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="B5" s="82" t="s">
-        <v>507</v>
+        <v>510</v>
       </c>
       <c r="C5" s="82" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
       <c r="D5" s="82"/>
       <c r="E5" s="82"/>
@@ -19369,13 +19430,13 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="82" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="B6" s="82" t="s">
-        <v>509</v>
+        <v>512</v>
       </c>
       <c r="C6" s="82" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
       <c r="D6" s="82"/>
       <c r="E6" s="82"/>
@@ -19400,13 +19461,13 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="82" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="B7" s="82" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
       <c r="C7" s="82" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="D7" s="82"/>
       <c r="E7" s="82"/>
@@ -19431,13 +19492,13 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="82" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="B8" s="82" t="s">
-        <v>513</v>
+        <v>516</v>
       </c>
       <c r="C8" s="82" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
       <c r="D8" s="82"/>
       <c r="E8" s="82"/>
@@ -19462,13 +19523,13 @@
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="82" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="B9" s="82" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
       <c r="C9" s="82" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="D9" s="82"/>
       <c r="E9" s="82"/>
@@ -19518,13 +19579,13 @@
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="82" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="B11" s="82" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="C11" s="82" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
       <c r="D11" s="82"/>
       <c r="E11" s="82"/>
@@ -19549,13 +19610,13 @@
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="82" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="B12" s="82" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="C12" s="82" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
       <c r="D12" s="82"/>
       <c r="E12" s="82"/>
@@ -19580,13 +19641,13 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="82" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="B13" s="82" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="C13" s="82" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="D13" s="82"/>
       <c r="E13" s="82"/>
@@ -19611,13 +19672,13 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="82" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="B14" s="82" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="C14" s="82" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="D14" s="82"/>
       <c r="E14" s="82"/>
@@ -19642,13 +19703,13 @@
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="82" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="B15" s="82" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="C15" s="82" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="D15" s="82"/>
       <c r="E15" s="82"/>
@@ -19673,13 +19734,13 @@
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="82" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="B16" s="82" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
       <c r="C16" s="82" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
       <c r="D16" s="82"/>
       <c r="E16" s="82"/>
@@ -19729,13 +19790,13 @@
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="82" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="B18" s="82" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="C18" s="82" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
       <c r="D18" s="82"/>
       <c r="E18" s="82"/>
@@ -19760,13 +19821,13 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="82" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="B19" s="82" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="C19" s="82" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
       <c r="D19" s="82"/>
       <c r="E19" s="82"/>
@@ -19791,13 +19852,13 @@
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="82" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="B20" s="82" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="C20" s="82" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="D20" s="82"/>
       <c r="E20" s="82"/>
@@ -19822,13 +19883,13 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="82" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="B21" s="82" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="C21" s="82" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="D21" s="82"/>
       <c r="E21" s="82"/>
@@ -19853,13 +19914,13 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="82" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="B22" s="82" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
       <c r="C22" s="82" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
       <c r="D22" s="82"/>
       <c r="E22" s="82"/>
@@ -19884,13 +19945,13 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="82" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="B23" s="82" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
       <c r="C23" s="82" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
       <c r="D23" s="82"/>
       <c r="E23" s="82"/>
@@ -19940,13 +20001,13 @@
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="82" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="B25" s="82" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="C25" s="82" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="D25" s="82"/>
       <c r="E25" s="82"/>
@@ -19971,13 +20032,13 @@
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="82" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="B26" s="82" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="C26" s="82" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="D26" s="82"/>
       <c r="E26" s="82"/>
@@ -20002,13 +20063,13 @@
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="82" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="B27" s="82" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
       <c r="C27" s="82" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
       <c r="D27" s="82"/>
       <c r="E27" s="82"/>
@@ -20033,13 +20094,13 @@
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="82" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="B28" s="82" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="C28" s="82" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c r="D28" s="82"/>
       <c r="E28" s="82"/>
@@ -20064,13 +20125,13 @@
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="82" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="B29" s="82" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="C29" s="82" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
       <c r="D29" s="82"/>
       <c r="E29" s="82"/>
@@ -20120,13 +20181,13 @@
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="82" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="B31" s="82" t="s">
-        <v>537</v>
+        <v>540</v>
       </c>
       <c r="C31" s="82" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="D31" s="82"/>
       <c r="E31" s="82"/>
@@ -20151,13 +20212,13 @@
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="82" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="B32" s="82" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
       <c r="C32" s="82" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="D32" s="82"/>
       <c r="E32" s="82"/>
@@ -20207,121 +20268,121 @@
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="B34" t="str">
         <f t="shared" ref="B34:B42" si="1">SUBSTITUTE(LOWER(SUBSTITUTE(SUBSTITUTE(C34, "(", ""), ")", "")), " ", "_")</f>
         <v>combined_oral_contraceptives</v>
       </c>
       <c r="C34" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="B35" t="str">
         <f t="shared" si="1"/>
         <v>progesterone_only_pills</v>
       </c>
       <c r="C35" t="s">
-        <v>541</v>
+        <v>544</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="B36" t="str">
         <f t="shared" si="1"/>
         <v>injectibles</v>
       </c>
       <c r="C36" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="B37" t="str">
         <f t="shared" si="1"/>
         <v>implants_1_rod</v>
       </c>
       <c r="C37" t="s">
-        <v>543</v>
+        <v>546</v>
       </c>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="B38" t="str">
         <f t="shared" si="1"/>
         <v>implants_2_rods</v>
       </c>
       <c r="C38" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="B39" t="str">
         <f t="shared" si="1"/>
         <v>iud</v>
       </c>
       <c r="C39" t="s">
-        <v>545</v>
+        <v>548</v>
       </c>
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="B40" t="str">
         <f t="shared" si="1"/>
         <v>condoms</v>
       </c>
       <c r="C40" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="B41" t="str">
         <f t="shared" si="1"/>
         <v>tubal_ligation</v>
       </c>
       <c r="C41" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="B42" t="str">
         <f t="shared" si="1"/>
         <v>cycle_beads</v>
       </c>
       <c r="C42" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="B43" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="C43" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
     </row>
     <row r="44" ht="15.75" customHeight="1">
@@ -20332,26 +20393,26 @@
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="B45" t="str">
         <f t="shared" si="2"/>
         <v>wants_to_get_pregnant</v>
       </c>
       <c r="C45" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="B46" t="str">
         <f t="shared" si="2"/>
         <v>did_not_want_fp</v>
       </c>
       <c r="C46" t="s">
-        <v>551</v>
+        <v>554</v>
       </c>
     </row>
     <row r="47" ht="15.75" customHeight="1">
@@ -20362,13 +20423,13 @@
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="96" t="s">
-        <v>552</v>
+        <v>555</v>
       </c>
       <c r="B48" s="96" t="s">
-        <v>553</v>
+        <v>556</v>
       </c>
       <c r="C48" s="96" t="s">
-        <v>554</v>
+        <v>557</v>
       </c>
       <c r="D48" s="96"/>
       <c r="E48" s="96"/>
@@ -20393,13 +20454,13 @@
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="96" t="s">
-        <v>552</v>
+        <v>555</v>
       </c>
       <c r="B49" s="96" t="s">
-        <v>555</v>
+        <v>558</v>
       </c>
       <c r="C49" s="96" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
       <c r="D49" s="96"/>
       <c r="E49" s="96"/>
@@ -20425,226 +20486,226 @@
     <row r="50" ht="15.75" customHeight="1"/>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
       <c r="B51" t="s">
-        <v>558</v>
+        <v>561</v>
       </c>
       <c r="C51" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
       <c r="B52" t="s">
-        <v>560</v>
+        <v>563</v>
       </c>
       <c r="C52" t="s">
-        <v>561</v>
+        <v>564</v>
       </c>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
       <c r="B53" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
       <c r="C53" t="s">
-        <v>563</v>
+        <v>566</v>
       </c>
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="A54" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
       <c r="B54" t="s">
-        <v>564</v>
+        <v>567</v>
       </c>
       <c r="C54" t="s">
-        <v>565</v>
+        <v>568</v>
       </c>
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
       <c r="B55" t="s">
-        <v>566</v>
+        <v>569</v>
       </c>
       <c r="C55" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
       <c r="B56" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="C56" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
     </row>
     <row r="57" ht="15.75" customHeight="1"/>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="96" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="B58" s="96" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="C58" s="96" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="96" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="B59" s="96" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
       <c r="C59" s="96" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="96" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="B60" s="96" t="s">
-        <v>573</v>
+        <v>576</v>
       </c>
       <c r="C60" s="96" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="96" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="B61" s="96" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="C61" s="96" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
     </row>
     <row r="62" ht="15.75" customHeight="1"/>
     <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="11" t="s">
-        <v>575</v>
+        <v>578</v>
       </c>
       <c r="B63" s="11" t="s">
-        <v>576</v>
+        <v>579</v>
       </c>
       <c r="C63" s="96" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="11" t="s">
-        <v>575</v>
+        <v>578</v>
       </c>
       <c r="B64" s="11" t="s">
-        <v>578</v>
+        <v>581</v>
       </c>
       <c r="C64" s="96" t="s">
-        <v>579</v>
+        <v>582</v>
       </c>
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="11" t="s">
-        <v>575</v>
+        <v>578</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>580</v>
+        <v>583</v>
       </c>
       <c r="C65" s="96" t="s">
-        <v>581</v>
+        <v>584</v>
       </c>
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="11" t="s">
-        <v>575</v>
+        <v>578</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>582</v>
+        <v>585</v>
       </c>
       <c r="C66" s="96" t="s">
-        <v>583</v>
+        <v>586</v>
       </c>
     </row>
     <row r="67" ht="15.75" customHeight="1">
       <c r="A67" s="11" t="s">
-        <v>575</v>
+        <v>578</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="C67" s="96" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
     </row>
     <row r="68" ht="15.75" customHeight="1"/>
     <row r="69" ht="15.75" customHeight="1">
       <c r="A69" t="s">
-        <v>584</v>
+        <v>587</v>
       </c>
       <c r="B69" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="C69" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="A70" t="s">
-        <v>584</v>
+        <v>587</v>
       </c>
       <c r="B70" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="C70" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
     </row>
     <row r="71" ht="15.75" customHeight="1"/>
     <row r="72" ht="15.75" customHeight="1">
       <c r="A72" t="s">
-        <v>585</v>
+        <v>588</v>
       </c>
       <c r="B72" t="s">
-        <v>586</v>
+        <v>589</v>
       </c>
       <c r="C72" s="97" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
     </row>
     <row r="73" ht="15.75" customHeight="1">
       <c r="A73" t="s">
-        <v>585</v>
+        <v>588</v>
       </c>
       <c r="B73" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="C73" t="s">
-        <v>588</v>
+        <v>591</v>
       </c>
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="A74" t="s">
-        <v>585</v>
+        <v>588</v>
       </c>
       <c r="B74" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="C74" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
     </row>
     <row r="75" ht="15.75" customHeight="1"/>

</xml_diff>